<commit_message>
Adding only 2020 data; creating tables & graphs
</commit_message>
<xml_diff>
--- a/data/pop_est.xlsx
+++ b/data/pop_est.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marytorres/Documents/covid19-vuln/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marytorres/Documents/covid19-vuln/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE65926-4F7C-F84F-810C-2F7AF2CAB79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07283A6F-A8DC-D54F-B742-148CA014A4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="18500" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="460" windowWidth="17420" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62:G64"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="188" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -471,7 +471,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="1">
-        <v>134494</v>
+        <v>129823</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -482,7 +482,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>46012</v>
+        <v>45839</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -493,7 +493,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>50077</v>
+        <v>49276</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -504,7 +504,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1">
-        <v>54276</v>
+        <v>53749</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -515,7 +515,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1">
-        <v>49742</v>
+        <v>50245</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -526,7 +526,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>38932</v>
+        <v>39656</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -537,7 +537,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="1">
-        <v>21241</v>
+        <v>22458</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1">
-        <v>189848</v>
+        <v>183233</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -559,7 +559,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>66675</v>
+        <v>66491</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>67120</v>
+        <v>66559</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -582,7 +582,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>73158</v>
+        <v>71945</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -595,7 +595,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1">
-        <v>64097</v>
+        <v>64989</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -608,7 +608,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="1">
-        <v>56610</v>
+        <v>48344</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="1">
-        <v>47291</v>
+        <v>30363</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -634,7 +634,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>97202</v>
+        <v>175814</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -647,7 +647,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="1">
-        <v>45137</v>
+        <v>63675</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -660,7 +660,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="1">
-        <v>70565</v>
+        <v>70029</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -673,7 +673,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1">
-        <v>71148</v>
+        <v>71834</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -686,7 +686,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="1">
-        <v>72395</v>
+        <v>66477</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -699,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="1">
-        <v>71188</v>
+        <v>49968</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -712,7 +712,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="1">
-        <v>65786</v>
+        <v>28762</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -725,7 +725,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="1">
-        <v>38590</v>
+        <v>38291</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -738,7 +738,7 @@
         <v>10</v>
       </c>
       <c r="C24" s="1">
-        <v>12900</v>
+        <v>12938</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -751,7 +751,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="1">
-        <v>14949</v>
+        <v>14600</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -764,7 +764,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="1">
-        <v>15744</v>
+        <v>15777</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -777,7 +777,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="1">
-        <v>13767</v>
+        <v>13725</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -790,7 +790,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="1">
-        <v>12235</v>
+        <v>12374</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -803,7 +803,7 @@
         <v>15</v>
       </c>
       <c r="C29" s="1">
-        <v>6661</v>
+        <v>7161</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -815,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="1">
-        <v>155060</v>
+        <v>149937</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -827,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="1">
-        <v>50207</v>
+        <v>49697</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -839,7 +839,7 @@
         <v>11</v>
       </c>
       <c r="C32" s="1">
-        <v>56497</v>
+        <v>55647</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -851,7 +851,7 @@
         <v>12</v>
       </c>
       <c r="C33" s="1">
-        <v>60947</v>
+        <v>60331</v>
       </c>
       <c r="F33" s="1"/>
     </row>
@@ -863,7 +863,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="1">
-        <v>59637</v>
+        <v>59463</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -875,7 +875,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="1">
-        <v>49239</v>
+        <v>50047</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -887,7 +887,7 @@
         <v>15</v>
       </c>
       <c r="C36" s="1">
-        <v>27900</v>
+        <v>29285</v>
       </c>
       <c r="F36" s="1"/>
     </row>
@@ -899,7 +899,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="1">
-        <v>227515</v>
+        <v>218946</v>
       </c>
       <c r="F37" s="1"/>
     </row>
@@ -911,7 +911,7 @@
         <v>10</v>
       </c>
       <c r="C38" s="1">
-        <v>79986</v>
+        <v>79089</v>
       </c>
       <c r="F38" s="1"/>
     </row>
@@ -923,7 +923,7 @@
         <v>11</v>
       </c>
       <c r="C39" s="1">
-        <v>84578</v>
+        <v>83026</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -935,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="C40" s="1">
-        <v>92430</v>
+        <v>90787</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -947,7 +947,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="1">
-        <v>84994</v>
+        <v>84748</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -959,7 +959,7 @@
         <v>14</v>
       </c>
       <c r="C42" s="1">
-        <v>66482</v>
+        <v>67908</v>
       </c>
       <c r="F42" s="1"/>
     </row>
@@ -971,7 +971,7 @@
         <v>15</v>
       </c>
       <c r="C43" s="1">
-        <v>46069</v>
+        <v>48014</v>
       </c>
       <c r="F43" s="1"/>
     </row>
@@ -983,7 +983,7 @@
         <v>16</v>
       </c>
       <c r="C44" s="1">
-        <v>167761</v>
+        <v>160873</v>
       </c>
       <c r="F44" s="1"/>
     </row>
@@ -995,7 +995,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="1">
-        <v>55126</v>
+        <v>54453</v>
       </c>
       <c r="F45" s="1"/>
     </row>
@@ -1007,7 +1007,7 @@
         <v>11</v>
       </c>
       <c r="C46" s="1">
-        <v>59247</v>
+        <v>58410</v>
       </c>
       <c r="F46" s="1"/>
     </row>
@@ -1019,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="C47" s="1">
-        <v>62249</v>
+        <v>61317</v>
       </c>
       <c r="F47" s="1"/>
     </row>
@@ -1031,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="1">
-        <v>61040</v>
+        <v>61071</v>
       </c>
       <c r="F48" s="1"/>
     </row>
@@ -1043,7 +1043,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="1">
-        <v>45115</v>
+        <v>46562</v>
       </c>
       <c r="F49" s="1"/>
     </row>
@@ -1055,7 +1055,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="1">
-        <v>24065</v>
+        <v>25337</v>
       </c>
       <c r="F50" s="1"/>
     </row>

</xml_diff>